<commit_message>
Número de iterações adicionado.
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -400,24 +400,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13">
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -431,25 +431,34 @@
         <v>1.1688304580369458e-10</v>
       </c>
       <c r="E2">
+        <v>315.0</v>
+      </c>
+      <c r="F2">
         <v>0.3</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.7</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>5.659205723365632e-6</v>
       </c>
-      <c r="H2">
-        <v>0.9</v>
-      </c>
       <c r="I2">
-        <v>0.9</v>
+        <v>2000.0</v>
       </c>
       <c r="J2">
+        <v>0.9</v>
+      </c>
+      <c r="K2">
+        <v>0.9</v>
+      </c>
+      <c r="L2">
         <v>7.223970139681705e-11</v>
       </c>
+      <c r="M2">
+        <v>1475.0</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -463,25 +472,34 @@
         <v>1.6156924085584347e-10</v>
       </c>
       <c r="E3">
+        <v>10000.0</v>
+      </c>
+      <c r="F3">
         <v>0.3</v>
       </c>
-      <c r="F3">
-        <v>0.9</v>
-      </c>
       <c r="G3">
+        <v>0.9</v>
+      </c>
+      <c r="H3">
         <v>1.1923789400597367e-10</v>
       </c>
-      <c r="H3">
+      <c r="I3">
+        <v>10000.0</v>
+      </c>
+      <c r="J3">
         <v>0.5</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0.7</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>1.1922524431928e-10</v>
       </c>
+      <c r="M3">
+        <v>10000.0</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -495,25 +513,34 @@
         <v>4.798857035674636e-14</v>
       </c>
       <c r="E4">
+        <v>20.0</v>
+      </c>
+      <c r="F4">
         <v>0.1</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.7</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1.4320294611095287e-13</v>
       </c>
-      <c r="H4">
-        <v>0.9</v>
-      </c>
       <c r="I4">
-        <v>0.9</v>
+        <v>31.0</v>
       </c>
       <c r="J4">
+        <v>0.9</v>
+      </c>
+      <c r="K4">
+        <v>0.9</v>
+      </c>
+      <c r="L4">
         <v>6.793908221948749e-17</v>
       </c>
+      <c r="M4">
+        <v>9.0</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -527,25 +554,34 @@
         <v>7.108658032496755e-15</v>
       </c>
       <c r="E5">
-        <v>0.3</v>
+        <v>9.0</v>
       </c>
       <c r="F5">
         <v>0.3</v>
       </c>
       <c r="G5">
+        <v>0.3</v>
+      </c>
+      <c r="H5">
         <v>3.0216589363745175e-14</v>
       </c>
-      <c r="H5">
+      <c r="I5">
+        <v>10.0</v>
+      </c>
+      <c r="J5">
         <v>0.5</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>0.5</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>8.163514646657e-15</v>
       </c>
+      <c r="M5">
+        <v>6.0</v>
+      </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -559,22 +595,31 @@
         <v>1.1102230246251565e-16</v>
       </c>
       <c r="E6">
+        <v>13.0</v>
+      </c>
+      <c r="F6">
         <v>0.1</v>
       </c>
-      <c r="F6">
-        <v>0.9</v>
-      </c>
       <c r="G6">
+        <v>0.9</v>
+      </c>
+      <c r="H6">
         <v>1.1102230246251565e-16</v>
       </c>
-      <c r="H6">
+      <c r="I6">
+        <v>16.0</v>
+      </c>
+      <c r="J6">
         <v>0.7</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>0.1</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>4.440892098500626e-16</v>
+      </c>
+      <c r="M6">
+        <v>85.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parâmetros de parada do gradiente padronizados.
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -428,10 +428,10 @@
         <v>0.001</v>
       </c>
       <c r="D2">
-        <v>1.1688304580369458e-10</v>
+        <v>1.944159978522072e-15</v>
       </c>
       <c r="E2">
-        <v>315.0</v>
+        <v>442.0</v>
       </c>
       <c r="F2">
         <v>0.3</v>
@@ -440,22 +440,22 @@
         <v>0.7</v>
       </c>
       <c r="H2">
-        <v>5.659205723365632e-6</v>
+        <v>5.6592057119481806e-6</v>
       </c>
       <c r="I2">
-        <v>2000.0</v>
+        <v>5000.0</v>
       </c>
       <c r="J2">
         <v>0.9</v>
       </c>
       <c r="K2">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="L2">
-        <v>7.223970139681705e-11</v>
+        <v>1.501992759363086e-13</v>
       </c>
       <c r="M2">
-        <v>1475.0</v>
+        <v>2869.0</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -463,40 +463,40 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="C3">
-        <v>9.999999999999999e-6</v>
+        <v>0.001</v>
       </c>
       <c r="D3">
-        <v>1.6156924085584347e-10</v>
+        <v>1.6156315450122798e-10</v>
       </c>
       <c r="E3">
-        <v>10000.0</v>
+        <v>1.0</v>
       </c>
       <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <v>0.5</v>
+      </c>
+      <c r="H3">
+        <v>5.960322351693935e-7</v>
+      </c>
+      <c r="I3">
+        <v>250.0</v>
+      </c>
+      <c r="J3">
         <v>0.3</v>
       </c>
-      <c r="G3">
+      <c r="K3">
         <v>0.9</v>
       </c>
-      <c r="H3">
-        <v>1.1923789400597367e-10</v>
-      </c>
-      <c r="I3">
-        <v>10000.0</v>
-      </c>
-      <c r="J3">
-        <v>0.5</v>
-      </c>
-      <c r="K3">
-        <v>0.7</v>
-      </c>
       <c r="L3">
-        <v>1.1922524431928e-10</v>
+        <v>5.957194087948522e-7</v>
       </c>
       <c r="M3">
-        <v>10000.0</v>
+        <v>278.0</v>
       </c>
     </row>
     <row r="4" spans="1:13">

</xml_diff>